<commit_message>
big boi graph for excel
</commit_message>
<xml_diff>
--- a/ma_results.xlsx
+++ b/ma_results.xlsx
@@ -302,7 +302,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for CAD_CHF and MA_24_64</a:t>
+              <a:t>Cum. Gains for CAD_CHF MA_24_64</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -852,7 +852,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for GBP_CAD and MA_64_256</a:t>
+              <a:t>Cum. Gains for GBP_CAD MA_64_256</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1000,7 +1000,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for GBP_CHF and MA_16_32</a:t>
+              <a:t>Cum. Gains for GBP_CHF MA_16_32</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1874,7 +1874,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for GBP_JPY and MA_8_64</a:t>
+              <a:t>Cum. Gains for GBP_JPY MA_8_64</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2454,7 +2454,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for GBP_NZD and MA_8_256</a:t>
+              <a:t>Cum. Gains for GBP_NZD MA_8_256</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2812,7 +2812,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for GBP_USD and MA_64_256</a:t>
+              <a:t>Cum. Gains for GBP_USD MA_64_256</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3002,7 +3002,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for NZD_CAD and MA_64_128</a:t>
+              <a:t>Cum. Gains for NZD_CAD MA_64_128</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3276,7 +3276,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for NZD_CHF and MA_32_256</a:t>
+              <a:t>Cum. Gains for NZD_CHF MA_32_256</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3538,7 +3538,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for NZD_JPY and MA_24_256</a:t>
+              <a:t>Cum. Gains for NZD_JPY MA_24_256</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3782,7 +3782,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for NZD_USD and MA_64_256</a:t>
+              <a:t>Cum. Gains for NZD_USD MA_64_256</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3972,7 +3972,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for USD_CAD and MA_8_32</a:t>
+              <a:t>Cum. Gains for USD_CAD MA_8_32</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4954,7 +4954,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for CAD_JPY and MA_16_32</a:t>
+              <a:t>Cum. Gains for CAD_JPY MA_16_32</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5762,7 +5762,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for USD_CHF and MA_16_64</a:t>
+              <a:t>Cum. Gains for USD_CHF MA_16_64</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6204,7 +6204,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for USD_JPY and MA_8_16</a:t>
+              <a:t>Cum. Gains for USD_JPY MA_8_16</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -7828,7 +7828,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for CHF_JPY and MA_32_64</a:t>
+              <a:t>Cum. Gains for CHF_JPY MA_32_64</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -8240,7 +8240,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for EUR_CAD and MA_8_32</a:t>
+              <a:t>Cum. Gains for EUR_CAD MA_8_32</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -9156,7 +9156,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for EUR_CHF and MA_4_128</a:t>
+              <a:t>Cum. Gains for EUR_CHF MA_4_128</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -9640,7 +9640,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for EUR_GBP and MA_64_128</a:t>
+              <a:t>Cum. Gains for EUR_GBP MA_64_128</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -9938,7 +9938,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for EUR_JPY and MA_8_32</a:t>
+              <a:t>Cum. Gains for EUR_JPY MA_8_32</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -10920,7 +10920,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for EUR_NZD and MA_32_96</a:t>
+              <a:t>Cum. Gains for EUR_NZD MA_32_96</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -11338,7 +11338,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CUM GAINS for EUR_USD and MA_64_128</a:t>
+              <a:t>Cum. Gains for EUR_USD MA_64_128</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -11601,10 +11601,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11636,10 +11636,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11671,10 +11671,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11706,10 +11706,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11741,10 +11741,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11776,10 +11776,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11811,10 +11811,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11846,10 +11846,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11881,10 +11881,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11916,10 +11916,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11951,10 +11951,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11986,10 +11986,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12021,10 +12021,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12056,10 +12056,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12091,10 +12091,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12126,10 +12126,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12161,10 +12161,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12196,10 +12196,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12231,10 +12231,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12266,10 +12266,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12301,10 +12301,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>